<commit_message>
cn-#22 Always using decimal over double
</commit_message>
<xml_diff>
--- a/test/Cactus.ExcelConverterTest/Features/ConverterTests.xlsx
+++ b/test/Cactus.ExcelConverterTest/Features/ConverterTests.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ExcelConverterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34ACFD1F-2D65-406C-8FCA-24B85C1A2852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882BA512-D8BC-4C81-A016-E5E36BD833CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2985" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exactly Matches" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateCount="250" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Given</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>DataGrid.xlsx</t>
+  </si>
+  <si>
+    <t>Formula Test</t>
+  </si>
+  <si>
+    <t>FormulaTest.xlsx</t>
+  </si>
+  <si>
+    <t>except empty lines</t>
   </si>
 </sst>
 </file>
@@ -143,9 +152,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E12"/>
+  <dimension ref="A2:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +483,7 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -489,6 +497,9 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -555,6 +566,22 @@
       <c r="E12" t="str">
         <f t="shared" si="1"/>
         <v>DataGrid.exp</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="D13" si="2">SUBSTITUTE(C13, ".xlsx", ".feature")</f>
+        <v>FormulaTest.feature</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" ref="E13" si="3">SUBSTITUTE(C13, ".xlsx", ".exp")</f>
+        <v>FormulaTest.exp</v>
       </c>
     </row>
   </sheetData>

</xml_diff>